<commit_message>
added arc159 volume bind for axis
</commit_message>
<xml_diff>
--- a/Excel Sketch.xlsx
+++ b/Excel Sketch.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\F14-Tomcat-Home-Cockpit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DIRECTEUR_PC2\Desktop\F14-Tomcat-Home-Cockpit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E063D0E-99CE-4CAC-9F87-10EDBBC144DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB56112-E2A2-4025-B806-16EE6E1E4295}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="26136" xr2:uid="{3BE12BD3-D686-44C7-AED3-1D6204E76DFE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BE12BD3-D686-44C7-AED3-1D6204E76DFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16461" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16463" uniqueCount="80">
   <si>
     <t>DEFINITION</t>
   </si>
@@ -260,6 +260,12 @@
   <si>
     <t>ICS SIDEWINDER VOLUMe</t>
   </si>
+  <si>
+    <t>action = device_commands.RADIO_UHF_VOL_STEP_Pilot, cockpit_deviceid = devices.ARC159, name = ('vol UHF grizzly')</t>
+  </si>
+  <si>
+    <t>ARC159 VOLUME</t>
+  </si>
 </sst>
 </file>
 
@@ -306,10 +312,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +438,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -725,26 +734,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EA02EE-AE90-4B73-B853-0E83CA661C12}">
-  <dimension ref="A16:XFD130"/>
+  <dimension ref="A33:XFD101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.21875" customWidth="1"/>
-    <col min="2" max="2" width="208.88671875" customWidth="1"/>
+    <col min="1" max="1" width="76.28515625" customWidth="1"/>
+    <col min="2" max="2" width="208.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -752,7 +759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -760,7 +767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -768,7 +775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -49922,7 +49929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -49930,7 +49937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -49938,7 +49945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -49946,7 +49953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -49954,7 +49961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -49962,7 +49969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -49970,7 +49977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:16384" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -49978,12 +49985,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -49991,7 +49998,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>77</v>
       </c>
@@ -49999,7 +50006,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -50007,7 +50014,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -50015,7 +50022,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -50023,15 +50030,23 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>76</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>27</v>
       </c>
@@ -50039,7 +50054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>24</v>
       </c>
@@ -50047,7 +50062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -50055,7 +50070,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -50063,7 +50078,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -50071,7 +50086,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>62</v>
       </c>
@@ -50079,179 +50094,161 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="113" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="120" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="121" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="126" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="128" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>